<commit_message>
i change my c study
</commit_message>
<xml_diff>
--- a/skillTable.xlsx
+++ b/skillTable.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuzewei/Documents/Git_repository/Learning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codeman/Documents/Learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="python核心编程" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="500">
   <si>
     <t>第2章  Python起步   31</t>
   </si>
@@ -3110,8 +3110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -3134,633 +3134,999 @@
       <c r="A2" t="s">
         <v>224</v>
       </c>
+      <c r="B2" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>225</v>
       </c>
+      <c r="B3" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>226</v>
       </c>
+      <c r="B4" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>227</v>
       </c>
+      <c r="B5" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>228</v>
       </c>
+      <c r="B6" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>229</v>
       </c>
+      <c r="B7" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>230</v>
       </c>
+      <c r="B8" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>231</v>
       </c>
+      <c r="B9" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>232</v>
       </c>
+      <c r="B10" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>233</v>
       </c>
+      <c r="B11" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>234</v>
       </c>
+      <c r="B12" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>235</v>
       </c>
+      <c r="B13" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>236</v>
       </c>
+      <c r="B14" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>237</v>
       </c>
+      <c r="B15" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B19" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B29" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B30" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B31" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B33" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B34" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B35" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B36" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B37" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B39" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B40" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B41" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B42" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B43" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B44" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B45" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B46" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B47" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B48" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B49" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B50" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B51" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B52" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B53" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B54" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B55" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B56" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B57" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B58" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B59" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B60" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B61" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B62" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B63" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B64" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B65" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B66" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B67" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B68" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B69" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B70" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B71" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B72" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B73" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B74" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B75" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B76" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B77" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B78" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B79" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B80" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A81" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B81" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B82" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B83" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B84" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B85" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B86" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B87" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B88" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B89" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B90" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B92" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A93" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B93" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A94" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B94" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A95" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B95" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B96" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B97" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B98" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B99" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A100" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B100" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A101" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B101" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A102" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B102" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A103" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B103" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A104" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B104" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A105" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B105" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A106" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B106" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A107" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B107" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A108" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B108" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B109" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B110" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B111" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B112" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B113" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B114" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B115" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B116" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B117" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B118" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B119" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B120" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B121" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B122" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B123" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
         <v>350</v>
       </c>
@@ -3806,7 +4172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
i delete the .DS_Store
</commit_message>
<xml_diff>
--- a/skillTable.xlsx
+++ b/skillTable.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="502">
   <si>
     <t>第2章  Python起步   31</t>
   </si>
@@ -1973,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="B113" sqref="B108:B113"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103:B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -2845,103 +2845,151 @@
       <c r="A108" t="s">
         <v>104</v>
       </c>
+      <c r="B108" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A109" t="s">
         <v>105</v>
       </c>
+      <c r="B109" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A110" t="s">
         <v>106</v>
       </c>
+      <c r="B110" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A111" t="s">
         <v>107</v>
       </c>
+      <c r="B111" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A112" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B112" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A113" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B113" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A114" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B114" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A115" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B115" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A116" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B116" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A117" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B117" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A118" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B118" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A119" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B119" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A120" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B120" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A121" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B121" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A122" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B122" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A123" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B123" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A125" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A126" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A127" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A128" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
i update my skill
</commit_message>
<xml_diff>
--- a/skillTable.xlsx
+++ b/skillTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="python核心编程" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="502">
   <si>
     <t>第2章  Python起步   31</t>
   </si>
@@ -1973,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103:B123"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -4546,8 +4546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -4654,6 +4654,9 @@
       <c r="B9">
         <v>27</v>
       </c>
+      <c r="C9" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -4662,6 +4665,9 @@
       <c r="B10">
         <v>29</v>
       </c>
+      <c r="C10" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -4670,6 +4676,9 @@
       <c r="B11">
         <v>30</v>
       </c>
+      <c r="C11" t="s">
+        <v>369</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>369</v>
       </c>
@@ -4681,6 +4690,9 @@
       <c r="B12">
         <v>38</v>
       </c>
+      <c r="C12" t="s">
+        <v>369</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>369</v>
       </c>
@@ -4692,6 +4704,9 @@
       <c r="B13">
         <v>45</v>
       </c>
+      <c r="C13" t="s">
+        <v>369</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>369</v>
       </c>
@@ -4703,6 +4718,9 @@
       <c r="B14">
         <v>53</v>
       </c>
+      <c r="C14" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
@@ -4711,6 +4729,9 @@
       <c r="B15">
         <v>60</v>
       </c>
+      <c r="C15" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
@@ -4719,168 +4740,231 @@
       <c r="B16">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C16" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>358</v>
       </c>
       <c r="B17">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C17" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>396</v>
       </c>
       <c r="B18">
         <v>74</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C18" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>397</v>
       </c>
       <c r="B19">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C19" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>398</v>
       </c>
       <c r="B20">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C20" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>399</v>
       </c>
       <c r="B21">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C21" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>400</v>
       </c>
       <c r="B22">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>401</v>
       </c>
       <c r="B23">
         <v>112</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C23" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>373</v>
       </c>
       <c r="B24">
         <v>119</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C24" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>402</v>
       </c>
       <c r="B25">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C25" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>403</v>
       </c>
       <c r="B26">
         <v>124</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C26" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>404</v>
       </c>
       <c r="B27">
         <v>126</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C27" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>405</v>
       </c>
       <c r="B28">
         <v>129</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>406</v>
       </c>
       <c r="B29">
         <v>131</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C29" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>407</v>
       </c>
       <c r="B30">
         <v>133</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C30" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>408</v>
       </c>
       <c r="B31">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C31" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>409</v>
       </c>
       <c r="B32">
         <v>135</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C32" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>410</v>
       </c>
       <c r="B33">
         <v>139</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C33" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>411</v>
       </c>
       <c r="B34">
         <v>140</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C34" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>412</v>
       </c>
       <c r="B35">
         <v>141</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C35" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>413</v>
       </c>
       <c r="B36">
         <v>147</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="C36" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>374</v>
       </c>
@@ -4888,7 +4972,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>414</v>
       </c>
@@ -4896,7 +4980,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>415</v>
       </c>
@@ -4904,7 +4988,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>416</v>
       </c>
@@ -4912,7 +4996,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>417</v>
       </c>
@@ -4920,7 +5004,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>418</v>
       </c>
@@ -4928,7 +5012,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>419</v>
       </c>
@@ -4936,7 +5020,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>359</v>
       </c>
@@ -4944,7 +5028,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>420</v>
       </c>
@@ -4952,7 +5036,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>421</v>
       </c>
@@ -4960,7 +5044,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>422</v>
       </c>
@@ -4968,7 +5052,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>423</v>
       </c>

</xml_diff>